<commit_message>
:bookmark: v0.1.1 - made daily features a wrapper around simple_features which gathers from duration. Added handling of overlapping activity and sleep periods, added more test
</commit_message>
<xml_diff>
--- a/tests/test_sleep_data.xlsx
+++ b/tests/test_sleep_data.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakre/Code/dgc/WellcomeLeap/mhealth_feature_generation/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50776C3-90EC-F842-93D5-D84C3834720F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DC2DD5-F7DF-DC4C-AC02-21F7011DB592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{D9B40E56-B593-D247-B317-A14C8FDAF4C2}"/>
+    <workbookView xWindow="1900" yWindow="1800" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{D9B40E56-B593-D247-B317-A14C8FDAF4C2}"/>
   </bookViews>
   <sheets>
     <sheet name="1_sleep_period_2_days" sheetId="1" r:id="rId1"/>
-    <sheet name="2_sleep_period_1_day" sheetId="2" r:id="rId2"/>
+    <sheet name="1_sleep_period_1_day_overlap" sheetId="5" r:id="rId2"/>
+    <sheet name="2_sleep_period_1_day" sheetId="2" r:id="rId3"/>
+    <sheet name="2_activity_overlap" sheetId="3" r:id="rId4"/>
+    <sheet name="6_heart_rate" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="21">
   <si>
     <t>user_id</t>
   </si>
@@ -88,6 +91,18 @@
   </si>
   <si>
     <t>Awake</t>
+  </si>
+  <si>
+    <t>source_device_model</t>
+  </si>
+  <si>
+    <t>Watch</t>
+  </si>
+  <si>
+    <t>ActiveEnergyBurned</t>
+  </si>
+  <si>
+    <t>HeartRate</t>
   </si>
 </sst>
 </file>
@@ -444,7 +459,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="A1:M8"/>
+      <selection sqref="A1:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,10 +710,154 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B350E1-8A81-1042-ACAE-11219762D260}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <v>44927.916666666664</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44928.25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44928.083333333336</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44928.25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44928.125</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44928.291666666664</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8443E48-CC3C-5A46-95E1-953536350F2F}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -871,4 +1030,301 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9463D09-89D2-324C-BAB4-354A1CE42FC6}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="A1:G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44927.416666666664</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44927.458333333336</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44927.4375</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44927.479166666664</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6FE30C-93A8-344E-9DAB-BE59459E28A9}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44927.416666666664</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44927.416666666664</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44927.4375</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44927.4375</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44927.438194444447</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44927.438194444447</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2">
+        <v>44927.438888888886</v>
+      </c>
+      <c r="D5" s="2">
+        <v>44927.438888888886</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44927.439583333333</v>
+      </c>
+      <c r="D6" s="2">
+        <v>44927.439583333333</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44927.44027777778</v>
+      </c>
+      <c r="D7" s="2">
+        <v>44927.44027777778</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44928.44027777778</v>
+      </c>
+      <c r="D8" s="2">
+        <v>44928.44027777778</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>